<commit_message>
line flows display done
</commit_message>
<xml_diff>
--- a/config_dummy.xlsx
+++ b/config_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>flaskSecret</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>mumbaiDemand</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,6 +891,11 @@
       </c>
       <c r="B43" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>